<commit_message>
Modified Excel document to include TrappedWater solution link
</commit_message>
<xml_diff>
--- a/DS-AlgoQns.xlsx
+++ b/DS-AlgoQns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\GitHub_Repo\DS-Algo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9902CF1-A3E0-4B31-B69F-888B4B364A76}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E50AD3F-E316-4AE2-B7E4-9B9CEF76C931}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Topic</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>O(N)</t>
+  </si>
+  <si>
+    <t>https://github.com/Gershon-Tadepalli/DS-Algo/blob/master/DS-AlgoPractice/DS-AlgoPractice/TrapWater.cs</t>
   </si>
 </sst>
 </file>
@@ -398,7 +401,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -407,7 +410,7 @@
     <col min="2" max="2" width="18.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.453125" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
     <col min="6" max="6" width="15.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
@@ -435,7 +438,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -447,6 +450,9 @@
       </c>
       <c r="D2" s="2" t="s">
         <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -458,6 +464,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{F7113BCA-8197-486B-838C-8A032A97DE5C}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{892EF7C3-9CB1-4814-92B0-37BEDF8C4E3C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2nd Day worked on StockSpan problem
</commit_message>
<xml_diff>
--- a/DS-AlgoQns.xlsx
+++ b/DS-AlgoQns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\GitHub_Repo\DS-Algo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E50AD3F-E316-4AE2-B7E4-9B9CEF76C931}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9191A043-D10F-4B50-89E3-23290AA85B76}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Topic</t>
   </si>
@@ -60,13 +60,32 @@
     <t>Tricky to find O(n)</t>
   </si>
   <si>
-    <t>Complexity</t>
-  </si>
-  <si>
     <t>O(N)</t>
   </si>
   <si>
     <t>https://github.com/Gershon-Tadepalli/DS-Algo/blob/master/DS-AlgoPractice/DS-AlgoPractice/TrapWater.cs</t>
+  </si>
+  <si>
+    <t>Best Time to buy&amp;sell stock</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/best-time-to-buy-and-sell-stock/</t>
+  </si>
+  <si>
+    <t>find sum of subarray( max+= arr[i]-arr[i-1])
+then find the largest subarray sum</t>
+  </si>
+  <si>
+    <t>Time Complexity</t>
+  </si>
+  <si>
+    <t>Space Complexity</t>
+  </si>
+  <si>
+    <t>O(1)</t>
+  </si>
+  <si>
+    <t>Easy but concept is sum of subarrays</t>
   </si>
 </sst>
 </file>
@@ -398,24 +417,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6328125" customWidth="1"/>
+    <col min="3" max="3" width="55.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.453125" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
-    <col min="6" max="6" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -435,10 +455,13 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>11</v>
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -452,19 +475,46 @@
         <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{F7113BCA-8197-486B-838C-8A032A97DE5C}"/>
     <hyperlink ref="E2" r:id="rId2" xr:uid="{892EF7C3-9CB1-4814-92B0-37BEDF8C4E3C}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{5D1D5171-8822-4140-B205-463764153C87}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added entry to Excel reference file
</commit_message>
<xml_diff>
--- a/DS-AlgoQns.xlsx
+++ b/DS-AlgoQns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\GitHub_Repo\DS-Algo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9191A043-D10F-4B50-89E3-23290AA85B76}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C285ED7-0687-4599-847E-F0B45871A609}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="21">
   <si>
     <t>Topic</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>O(N)</t>
-  </si>
-  <si>
-    <t>https://github.com/Gershon-Tadepalli/DS-Algo/blob/master/DS-AlgoPractice/DS-AlgoPractice/TrapWater.cs</t>
   </si>
   <si>
     <t>Best Time to buy&amp;sell stock</t>
@@ -86,13 +83,19 @@
   </si>
   <si>
     <t>Easy but concept is sum of subarrays</t>
+  </si>
+  <si>
+    <t>https://github.com/Gershon-Tadepalli/DS-Algo/blob/master/DS-AlgoPractice/DS-AlgoLibrary/Arrays/TrapWater.cs</t>
+  </si>
+  <si>
+    <t>https://github.com/Gershon-Tadepalli/DS-Algo/blob/master/DS-AlgoPractice/DS-AlgoLibrary/Arrays/StockSpan.cs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +107,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -130,12 +140,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -419,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -429,36 +440,36 @@
     <col min="2" max="2" width="23.6328125" customWidth="1"/>
     <col min="3" max="3" width="55.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.453125" customWidth="1"/>
-    <col min="5" max="5" width="29" customWidth="1"/>
+    <col min="5" max="5" width="54.6328125" customWidth="1"/>
     <col min="6" max="6" width="31.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.7265625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="H1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -475,7 +486,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -484,7 +495,7 @@
         <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -492,22 +503,25 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>15</v>
+      <c r="E3" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -515,6 +529,7 @@
     <hyperlink ref="C2" r:id="rId1" xr:uid="{F7113BCA-8197-486B-838C-8A032A97DE5C}"/>
     <hyperlink ref="E2" r:id="rId2" xr:uid="{892EF7C3-9CB1-4814-92B0-37BEDF8C4E3C}"/>
     <hyperlink ref="C3" r:id="rId3" xr:uid="{5D1D5171-8822-4140-B205-463764153C87}"/>
+    <hyperlink ref="E3" r:id="rId4" xr:uid="{8AF0207A-458D-47C5-A1F5-9BFCF5467F56}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Removing duplicates from sorted Array
</commit_message>
<xml_diff>
--- a/DS-AlgoQns.xlsx
+++ b/DS-AlgoQns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\GitHub_Repo\DS-Algo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C285ED7-0687-4599-847E-F0B45871A609}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1593188F-DB60-4B38-958F-FDA660923460}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Topic</t>
   </si>
@@ -89,6 +89,16 @@
   </si>
   <si>
     <t>https://github.com/Gershon-Tadepalli/DS-Algo/blob/master/DS-AlgoPractice/DS-AlgoLibrary/Arrays/StockSpan.cs</t>
+  </si>
+  <si>
+    <t>Remove Duplicates from Sorted Array</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-easy/92/array/727/</t>
+  </si>
+  <si>
+    <t>Use two pointers :
+whenever unique element is found store it at next index,for duplicates skip them.</t>
   </si>
 </sst>
 </file>
@@ -428,17 +438,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A3" sqref="A3:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.6328125" customWidth="1"/>
-    <col min="3" max="3" width="55.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.7265625" customWidth="1"/>
     <col min="4" max="4" width="38.453125" customWidth="1"/>
     <col min="5" max="5" width="54.6328125" customWidth="1"/>
     <col min="6" max="6" width="31.81640625" bestFit="1" customWidth="1"/>
@@ -524,12 +534,27 @@
         <v>17</v>
       </c>
     </row>
+    <row r="4" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{F7113BCA-8197-486B-838C-8A032A97DE5C}"/>
     <hyperlink ref="E2" r:id="rId2" xr:uid="{892EF7C3-9CB1-4814-92B0-37BEDF8C4E3C}"/>
     <hyperlink ref="C3" r:id="rId3" xr:uid="{5D1D5171-8822-4140-B205-463764153C87}"/>
     <hyperlink ref="E3" r:id="rId4" xr:uid="{8AF0207A-458D-47C5-A1F5-9BFCF5467F56}"/>
+    <hyperlink ref="C4" r:id="rId5" xr:uid="{BA76E1DF-82A0-416B-9867-4C68083F381F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Entry to excel file
</commit_message>
<xml_diff>
--- a/DS-AlgoQns.xlsx
+++ b/DS-AlgoQns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\GitHub_Repo\DS-Algo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1593188F-DB60-4B38-958F-FDA660923460}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8DB478-8809-486A-B571-B7948AA728FB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>Topic</t>
   </si>
@@ -99,6 +99,12 @@
   <si>
     <t>Use two pointers :
 whenever unique element is found store it at next index,for duplicates skip them.</t>
+  </si>
+  <si>
+    <t>https://github.com/Gershon-Tadepalli/DS-Algo/blob/master/DS-AlgoPractice/DS-AlgoLibrary/Arrays/RemoveDuplicatesOfSortedArray.cs</t>
+  </si>
+  <si>
+    <t>Easy just modify given array to store unique elements by using 2 pointers(variables)</t>
   </si>
 </sst>
 </file>
@@ -440,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -547,6 +553,18 @@
       <c r="D4" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="E4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -555,6 +573,7 @@
     <hyperlink ref="C3" r:id="rId3" xr:uid="{5D1D5171-8822-4140-B205-463764153C87}"/>
     <hyperlink ref="E3" r:id="rId4" xr:uid="{8AF0207A-458D-47C5-A1F5-9BFCF5467F56}"/>
     <hyperlink ref="C4" r:id="rId5" xr:uid="{BA76E1DF-82A0-416B-9867-4C68083F381F}"/>
+    <hyperlink ref="E4" r:id="rId6" xr:uid="{E4990DC1-4F28-45A9-8B15-59CE6C02C6CB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
first Bad version problem
</commit_message>
<xml_diff>
--- a/DS-AlgoQns.xlsx
+++ b/DS-AlgoQns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\GitHub_Repo\DS-Algo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83ADC8FF-A116-45F8-8E18-359773262FDF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA83030-C191-43C2-B476-82C2701EE820}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
   <si>
     <t>Topic</t>
   </si>
@@ -123,6 +123,39 @@
   </si>
   <si>
     <t>https://github.com/Gershon-Tadepalli/DS-Algo/blob/master/DS-AlgoPractice/DS-AlgoLibrary/Strings/ReverseAString.cs</t>
+  </si>
+  <si>
+    <t>Valid Palindrome</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-easy/127/strings/883/</t>
+  </si>
+  <si>
+    <t>Use two pointer approach if characters are equal or not</t>
+  </si>
+  <si>
+    <t>https://github.com/Gershon-Tadepalli/DS-Algo/blob/master/DS-AlgoPractice/DS-AlgoLibrary/Strings/Palindrome.cs</t>
+  </si>
+  <si>
+    <t>Easy - make sure to skip any non alphanumeric characters</t>
+  </si>
+  <si>
+    <t>Searching And Sorting</t>
+  </si>
+  <si>
+    <t>First Bad version</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-easy/96/sorting-and-searching/774/</t>
+  </si>
+  <si>
+    <t>Use Binary search approach to find bad version until both pointers resolve to 1</t>
+  </si>
+  <si>
+    <t>O(logN)</t>
+  </si>
+  <si>
+    <t>Easy - Binary Search</t>
   </si>
 </sst>
 </file>
@@ -462,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -610,6 +643,55 @@
         <v>17</v>
       </c>
     </row>
+    <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{F7113BCA-8197-486B-838C-8A032A97DE5C}"/>
@@ -620,8 +702,11 @@
     <hyperlink ref="E4" r:id="rId6" xr:uid="{E4990DC1-4F28-45A9-8B15-59CE6C02C6CB}"/>
     <hyperlink ref="C5" r:id="rId7" xr:uid="{DF01A8BB-F6FD-4F9A-BFCD-72A91824C389}"/>
     <hyperlink ref="E5" r:id="rId8" xr:uid="{1E4BE6AF-7418-4352-9995-EFB5571F82E9}"/>
+    <hyperlink ref="C6" r:id="rId9" xr:uid="{B982EC62-1481-4CDA-B73C-D44885B9D8D9}"/>
+    <hyperlink ref="E6" r:id="rId10" xr:uid="{7C9DAC70-1FE9-4120-88AB-75C743D592DE}"/>
+    <hyperlink ref="C7" r:id="rId11" xr:uid="{2B564D74-14A2-4E25-B209-F00B1ABDA1A9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId9"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added entry to excel
</commit_message>
<xml_diff>
--- a/DS-AlgoQns.xlsx
+++ b/DS-AlgoQns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\GitHub_Repo\DS-Algo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA83030-C191-43C2-B476-82C2701EE820}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3DC487-7462-4180-989F-4F9C38167C09}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
   <si>
     <t>Topic</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>Easy - Binary Search</t>
+  </si>
+  <si>
+    <t>https://github.com/Gershon-Tadepalli/DS-Algo/blob/master/DS-AlgoPractice/DS-AlgoLibrary/SortingAndSearching/FirstBadVersion.cs</t>
   </si>
 </sst>
 </file>
@@ -497,7 +500,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -682,6 +685,9 @@
       <c r="D7" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="E7" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F7" t="s">
         <v>42</v>
       </c>
@@ -705,8 +711,9 @@
     <hyperlink ref="C6" r:id="rId9" xr:uid="{B982EC62-1481-4CDA-B73C-D44885B9D8D9}"/>
     <hyperlink ref="E6" r:id="rId10" xr:uid="{7C9DAC70-1FE9-4120-88AB-75C743D592DE}"/>
     <hyperlink ref="C7" r:id="rId11" xr:uid="{2B564D74-14A2-4E25-B209-F00B1ABDA1A9}"/>
+    <hyperlink ref="E7" r:id="rId12" xr:uid="{360B76D8-621F-4A47-BDD5-0E49B55C345C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId12"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
reverse a linked list
</commit_message>
<xml_diff>
--- a/DS-AlgoQns.xlsx
+++ b/DS-AlgoQns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\GitHub_Repo\DS-Algo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3DC487-7462-4180-989F-4F9C38167C09}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F79A80-6317-4B3E-8B31-6A4ABD1470C1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
   <si>
     <t>Topic</t>
   </si>
@@ -159,6 +159,18 @@
   </si>
   <si>
     <t>https://github.com/Gershon-Tadepalli/DS-Algo/blob/master/DS-AlgoPractice/DS-AlgoLibrary/SortingAndSearching/FirstBadVersion.cs</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/explore/interview/card/top-interview-questions-easy/93/linked-list/560/</t>
+  </si>
+  <si>
+    <t>Reverse a Linked List</t>
+  </si>
+  <si>
+    <t>Linked List</t>
+  </si>
+  <si>
+    <t>Easy - keep track of current and previous node</t>
   </si>
 </sst>
 </file>
@@ -498,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -698,6 +710,26 @@
         <v>17</v>
       </c>
     </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{F7113BCA-8197-486B-838C-8A032A97DE5C}"/>
@@ -712,8 +744,9 @@
     <hyperlink ref="E6" r:id="rId10" xr:uid="{7C9DAC70-1FE9-4120-88AB-75C743D592DE}"/>
     <hyperlink ref="C7" r:id="rId11" xr:uid="{2B564D74-14A2-4E25-B209-F00B1ABDA1A9}"/>
     <hyperlink ref="E7" r:id="rId12" xr:uid="{360B76D8-621F-4A47-BDD5-0E49B55C345C}"/>
+    <hyperlink ref="C8" r:id="rId13" xr:uid="{9DE480AC-D1E2-4A22-9A75-A01E57A78D18}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId13"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Recursive approach to solve reverse a linked list
</commit_message>
<xml_diff>
--- a/DS-AlgoQns.xlsx
+++ b/DS-AlgoQns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\GitHub_Repo\DS-Algo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75469ED7-29F2-4BCD-9E49-42282AA2DB53}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D82F8C-F62C-49E4-87C3-526E8B71336F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
   <si>
     <t>Topic</t>
   </si>
@@ -174,6 +174,11 @@
   </si>
   <si>
     <t>https://github.com/Gershon-Tadepalli/DS-Algo/blob/master/DS-AlgoPractice/DS-AlgoLibrary/LinkedList/ReverseALinkedList.cs</t>
+  </si>
+  <si>
+    <t>1. Use Iterative approach with 2 ref's prev and curr
+2. Use Recursive approach by reversing rest n-1 nodes and linking head node
+3. Use Recursive approach by reversing first n-1 nodes</t>
   </si>
 </sst>
 </file>
@@ -515,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C10" sqref="C8:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -713,7 +718,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="87" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -722,6 +727,9 @@
       </c>
       <c r="C8" s="1" t="s">
         <v>44</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>48</v>

</xml_diff>